<commit_message>
Updated results for English condition after removing PUD
</commit_message>
<xml_diff>
--- a/results/acl-en/baselines_pos.xlsx
+++ b/results/acl-en/baselines_pos.xlsx
@@ -456,7 +456,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>0.1907189727611764</v>
+        <v>0.1982921009669723</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -464,7 +464,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0.1961952255621739</v>
+        <v>0.2118068965517241</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -472,7 +472,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>0.203014482990906</v>
+        <v>0.1805458229957766</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -504,7 +504,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>0.2526266635535839</v>
+        <v>0.2757242757242757</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -536,7 +536,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>0.2358186397984887</v>
+        <v>0.216893039049236</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -544,7 +544,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>0.266889970296404</v>
+        <v>0.2738805263656158</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -568,7 +568,7 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>0.2425955741940315</v>
+        <v>0.2832591683289857</v>
       </c>
     </row>
     <row r="17" spans="1:2">

</xml_diff>